<commit_message>
Updated CHE model - 2025-08-15 02:52
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SysSettings.xlsx
+++ b/VerveStacks_CHE/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9348A2-C26D-4576-A051-F3D6547227A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFD584F-EF7F-4925-8BC2-62CDD69B9DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system_settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="213">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -3007,7 +3007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4236,9 +4236,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EBD23C-EA82-4040-97D7-F532F0547462}">
-  <dimension ref="A2:P93"/>
+  <dimension ref="A2:P95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J95" sqref="J95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="11.65"/>
   <cols>
@@ -5301,14 +5303,20 @@
       <c r="B51" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>196</v>
+      <c r="G51" s="11" t="str">
+        <f>G46</f>
+        <v>G_CUREX</v>
+      </c>
+      <c r="I51" s="11" t="str">
+        <f t="shared" ref="I51:K51" si="0">I46</f>
+        <v>USD20</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="K51" s="11">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.98960000000000004</v>
       </c>
     </row>
     <row r="52" spans="2:11" ht="13.15">
@@ -5319,7 +5327,7 @@
         <v>196</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K52" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5333,7 +5341,7 @@
         <v>196</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K53" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5347,7 +5355,7 @@
         <v>196</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K54" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5358,7 +5366,7 @@
         <v>196</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K55" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5369,7 +5377,7 @@
         <v>196</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K56" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5380,7 +5388,7 @@
         <v>196</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K57" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5391,7 +5399,7 @@
         <v>196</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K58" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5402,7 +5410,7 @@
         <v>196</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K59" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5413,7 +5421,7 @@
         <v>196</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K60" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5424,7 +5432,7 @@
         <v>196</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K61" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5435,7 +5443,7 @@
         <v>196</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K62" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5446,7 +5454,7 @@
         <v>196</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K63" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5457,7 +5465,7 @@
         <v>196</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K64" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5468,7 +5476,7 @@
         <v>196</v>
       </c>
       <c r="J65" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K65" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5479,7 +5487,7 @@
         <v>196</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K66" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5490,7 +5498,7 @@
         <v>196</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K67" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5501,7 +5509,7 @@
         <v>196</v>
       </c>
       <c r="J68" s="11" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="K68" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5512,7 +5520,7 @@
         <v>196</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="K69" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5523,7 +5531,7 @@
         <v>196</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K70" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5534,7 +5542,7 @@
         <v>196</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K71" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5545,7 +5553,7 @@
         <v>196</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K72" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5556,7 +5564,7 @@
         <v>196</v>
       </c>
       <c r="J73" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K73" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5567,7 +5575,7 @@
         <v>196</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K74" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5578,7 +5586,7 @@
         <v>196</v>
       </c>
       <c r="J75" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K75" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5589,7 +5597,7 @@
         <v>196</v>
       </c>
       <c r="J76" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K76" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5600,7 +5608,7 @@
         <v>196</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K77" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5611,7 +5619,7 @@
         <v>196</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K78" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5622,7 +5630,7 @@
         <v>196</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K79" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5633,7 +5641,7 @@
         <v>196</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K80" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5644,7 +5652,7 @@
         <v>196</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K81" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5655,7 +5663,7 @@
         <v>196</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K82" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5666,7 +5674,7 @@
         <v>196</v>
       </c>
       <c r="J83" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K83" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5677,7 +5685,7 @@
         <v>196</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K84" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5688,7 +5696,7 @@
         <v>196</v>
       </c>
       <c r="J85" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K85" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5699,7 +5707,7 @@
         <v>196</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K86" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5710,7 +5718,7 @@
         <v>196</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K87" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5721,7 +5729,7 @@
         <v>196</v>
       </c>
       <c r="J88" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K88" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5732,7 +5740,7 @@
         <v>196</v>
       </c>
       <c r="J89" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K89" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5743,7 +5751,7 @@
         <v>196</v>
       </c>
       <c r="J90" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K90" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5754,7 +5762,7 @@
         <v>196</v>
       </c>
       <c r="J91" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K91" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5765,7 +5773,7 @@
         <v>196</v>
       </c>
       <c r="J92" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K92" s="11">
         <v>7.0000000000000007E-2</v>
@@ -5776,9 +5784,32 @@
         <v>196</v>
       </c>
       <c r="J93" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K93" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="7:11">
+      <c r="G94" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="J94" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="K93" s="11">
+      <c r="K94" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="7:11">
+      <c r="G95" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="J95" s="11" t="str">
+        <f>J51</f>
+        <v>USD21_alt</v>
+      </c>
+      <c r="K95" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>

</xml_diff>